<commit_message>
Brushed diagram up, added it as pdf
</commit_message>
<xml_diff>
--- a/exp2/data/data.xlsx
+++ b/exp2/data/data.xlsx
@@ -269,7 +269,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-8.1996719160104994E-2"/>
-                  <c:y val="2.1372849227179959E-3"/>
+                  <c:y val="2.1372849227179968E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -348,8 +348,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.10133661417322837"/>
-                  <c:y val="-0.18220472440944888"/>
+                  <c:x val="0.10133661417322838"/>
+                  <c:y val="-0.1822047244094489"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -410,26 +410,26 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="107620608"/>
-        <c:axId val="107622400"/>
+        <c:axId val="99096832"/>
+        <c:axId val="99102720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107620608"/>
+        <c:axId val="99096832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
-          <c:min val="0.30000000000000016"/>
+          <c:min val="0.30000000000000021"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107622400"/>
+        <c:crossAx val="99102720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107622400"/>
+        <c:axId val="99102720"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -440,7 +440,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107620608"/>
+        <c:crossAx val="99096832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -453,7 +453,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -463,6 +463,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-CH"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>Resonance Frequencies</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -471,7 +489,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>K_1</c:v>
+            <c:v>1.5 kp</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -570,7 +588,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>K_2</c:v>
+            <c:v>3 kp</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -669,7 +687,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Expected K_1</c:v>
+            <c:v>Expected 1.5 kp</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875">
@@ -740,7 +758,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Expected K_2</c:v>
+            <c:v>Expected 3 kp</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875">
@@ -807,25 +825,43 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="107648512"/>
-        <c:axId val="107650048"/>
+        <c:axId val="99137792"/>
+        <c:axId val="100798464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107648512"/>
+        <c:axId val="99137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.35000000000000009"/>
+          <c:max val="0.35000000000000014"/>
           <c:min val="-0.5"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Log_10(lambda)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107650048"/>
+        <c:crossAx val="100798464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107650048"/>
+        <c:axId val="100798464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.8"/>
@@ -833,9 +869,27 @@
         </c:scaling>
         <c:axPos val="r"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Log_10(f)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107648512"/>
+        <c:crossAx val="99137792"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -848,8 +902,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
+    <c:pageMargins b="1.05277777777778" l="0.78749999999999998" r="0.78749999999999998" t="1.05277777777778" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -888,16 +942,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1206,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
@@ -1922,7 +1976,7 @@
         <v>2.0972573096934197</v>
       </c>
       <c r="H38">
-        <f t="shared" ref="G38:K38" si="10">LOG10(H9)</f>
+        <f t="shared" ref="H38:K38" si="10">LOG10(H9)</f>
         <v>2.2716093013788319</v>
       </c>
       <c r="I38">

</xml_diff>

<commit_message>
new pdf plus some further work
</commit_message>
<xml_diff>
--- a/exp2/data/data.xlsx
+++ b/exp2/data/data.xlsx
@@ -269,7 +269,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-8.1996719160104994E-2"/>
-                  <c:y val="2.1372849227179968E-3"/>
+                  <c:y val="2.1372849227179981E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -348,7 +348,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.10133661417322838"/>
+                  <c:x val="0.1013366141732284"/>
                   <c:y val="-0.1822047244094489"/>
                 </c:manualLayout>
               </c:layout>
@@ -410,26 +410,26 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="99096832"/>
-        <c:axId val="99102720"/>
+        <c:axId val="94705920"/>
+        <c:axId val="94711808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99096832"/>
+        <c:axId val="94705920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
-          <c:min val="0.30000000000000021"/>
+          <c:min val="0.30000000000000027"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99102720"/>
+        <c:crossAx val="94711808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99102720"/>
+        <c:axId val="94711808"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -440,7 +440,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99096832"/>
+        <c:crossAx val="94705920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -453,7 +453,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -825,14 +825,14 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="99137792"/>
-        <c:axId val="100798464"/>
+        <c:axId val="94759168"/>
+        <c:axId val="99365248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99137792"/>
+        <c:axId val="94759168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.35000000000000014"/>
+          <c:max val="0.3500000000000002"/>
           <c:min val="-0.5"/>
         </c:scaling>
         <c:axPos val="b"/>
@@ -847,7 +847,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Log_10(lambda)</a:t>
+                  <a:t>Log_10(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>λ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -856,12 +864,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100798464"/>
+        <c:crossAx val="99365248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100798464"/>
+        <c:axId val="99365248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.8"/>
@@ -889,7 +897,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99137792"/>
+        <c:crossAx val="94759168"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -902,7 +910,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.05277777777778" l="0.78749999999999998" r="0.78749999999999998" t="1.05277777777778" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="1.05277777777778" l="0.78749999999999998" r="0.78749999999999998" t="1.05277777777778" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1260,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>

</xml_diff>